<commit_message>
Implement new schematic changes
</commit_message>
<xml_diff>
--- a/src/main/resources/ru/avem/pult/app/form2.xlsx
+++ b/src/main/resources/ru/avem/pult/app/form2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\IdeaProjects\viu-l-pc\src\main\resources\ru\avem\highvoltage\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\IdeaProjects\pult\src\main\resources\ru\avem\pult\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Протокол испытания №</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>дата</t>
-  </si>
-  <si>
-    <t>ПАО "Сургутнефтегаз"</t>
   </si>
   <si>
     <t>Испытатель:</t>
@@ -209,15 +206,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -226,6 +214,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,7 +507,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -521,85 +518,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="16"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="B4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="B5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -624,22 +619,22 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -648,109 +643,109 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="11"/>
+      <c r="A20" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="16"/>
       <c r="E20" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="16" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="11"/>
+      <c r="D21" s="16"/>
       <c r="E21" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1732,27 +1727,27 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A18:F18"/>
     <mergeCell ref="A22:F22"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>